<commit_message>
Clean up whitespace on Namibia
</commit_message>
<xml_diff>
--- a/data/xlsx/NA.xlsx
+++ b/data/xlsx/NA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B54E854-A22E-EC49-9C69-3E80FC5B500C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355B0589-CC92-B944-BC81-203A71AF27B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33140" yWindow="-740" windowWidth="34060" windowHeight="16500" xr2:uid="{223A3816-2ADA-D240-8330-DCA73EC25BC7}"/>
   </bookViews>
@@ -695,9 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C7B6504-01EB-1E42-ADCE-10FA03C71DF1}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>